<commit_message>
[PHOENIX-5854] changrs in trade license
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/tradeLicenseTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/tradeLicenseTestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
   <si>
     <t>dataName</t>
   </si>
@@ -153,9 +153,6 @@
     <t>TL/08360/2016</t>
   </si>
   <si>
-    <t>Veterinary Trades</t>
-  </si>
-  <si>
     <t xml:space="preserve">01987-2017-HB </t>
   </si>
   <si>
@@ -165,7 +162,7 @@
     <t>Permanent</t>
   </si>
   <si>
-    <t>01/03/2017</t>
+    <t>30/03/2017</t>
   </si>
 </sst>
 </file>
@@ -673,7 +670,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -723,13 +720,13 @@
         <v>26</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>27</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F2" s="7">
         <v>100</v>
@@ -738,7 +735,7 @@
         <v>28</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -746,7 +743,7 @@
         <v>27</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -835,7 +832,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -862,8 +859,8 @@
       <c r="B2" t="s">
         <v>38</v>
       </c>
-      <c r="C2" t="s">
-        <v>44</v>
+      <c r="C2" s="7" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -899,7 +896,7 @@
         <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>